<commit_message>
example policy run outputs
</commit_message>
<xml_diff>
--- a/param_files/calibration_code_results/2021_09_22/IPT_inititation_df.xlsx
+++ b/param_files/calibration_code_results/2021_09_22/IPT_inititation_df.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/param_files/calibration_code_results/2021_09_22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56386416-F180-224C-93A2-EE9DA7BF705C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA58A14-E4FA-A94B-A40C-F8EB56B68E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21460" yWindow="0" windowWidth="14380" windowHeight="18060" xr2:uid="{0D5B4E24-E2BC-434F-9926-FFC45EE0525A}"/>
+    <workbookView xWindow="15640" yWindow="300" windowWidth="14380" windowHeight="18060" activeTab="1" xr2:uid="{0D5B4E24-E2BC-434F-9926-FFC45EE0525A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="warm_up" sheetId="1" r:id="rId1"/>
+    <sheet name="policies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="10">
   <si>
     <t>Male</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>POLICY_ID</t>
   </si>
 </sst>
 </file>
@@ -418,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5232D7E8-72AD-0640-BDF6-FB7E1791E5B5}">
   <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1687,7 +1691,7 @@
       </c>
       <c r="D73" s="1">
         <f>(D85-D72)/(A85-A72)</f>
-        <v>3.0769230769230769E-3</v>
+        <v>0</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
@@ -1705,7 +1709,7 @@
       </c>
       <c r="D74" s="1">
         <f>$D$73+D73</f>
-        <v>6.1538461538461538E-3</v>
+        <v>0</v>
       </c>
       <c r="E74" t="s">
         <v>8</v>
@@ -1723,7 +1727,7 @@
       </c>
       <c r="D75" s="1">
         <f t="shared" ref="D75:D84" si="2">$D$73+D74</f>
-        <v>9.2307692307692299E-3</v>
+        <v>0</v>
       </c>
       <c r="E75" t="s">
         <v>8</v>
@@ -1741,7 +1745,7 @@
       </c>
       <c r="D76" s="1">
         <f t="shared" si="2"/>
-        <v>1.2307692307692308E-2</v>
+        <v>0</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
@@ -1759,7 +1763,7 @@
       </c>
       <c r="D77" s="1">
         <f t="shared" si="2"/>
-        <v>1.5384615384615385E-2</v>
+        <v>0</v>
       </c>
       <c r="E77" t="s">
         <v>8</v>
@@ -1777,7 +1781,7 @@
       </c>
       <c r="D78" s="1">
         <f t="shared" si="2"/>
-        <v>1.8461538461538463E-2</v>
+        <v>0</v>
       </c>
       <c r="E78" t="s">
         <v>8</v>
@@ -1795,7 +1799,7 @@
       </c>
       <c r="D79" s="1">
         <f t="shared" si="2"/>
-        <v>2.1538461538461541E-2</v>
+        <v>0</v>
       </c>
       <c r="E79" t="s">
         <v>8</v>
@@ -1813,7 +1817,7 @@
       </c>
       <c r="D80" s="1">
         <f t="shared" si="2"/>
-        <v>2.4615384615384619E-2</v>
+        <v>0</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -1831,7 +1835,7 @@
       </c>
       <c r="D81" s="1">
         <f t="shared" si="2"/>
-        <v>2.7692307692307697E-2</v>
+        <v>0</v>
       </c>
       <c r="E81" t="s">
         <v>8</v>
@@ -1849,7 +1853,7 @@
       </c>
       <c r="D82" s="1">
         <f t="shared" si="2"/>
-        <v>3.0769230769230774E-2</v>
+        <v>0</v>
       </c>
       <c r="E82" t="s">
         <v>8</v>
@@ -1867,7 +1871,7 @@
       </c>
       <c r="D83" s="1">
         <f t="shared" si="2"/>
-        <v>3.3846153846153852E-2</v>
+        <v>0</v>
       </c>
       <c r="E83" t="s">
         <v>8</v>
@@ -1885,7 +1889,7 @@
       </c>
       <c r="D84" s="1">
         <f t="shared" si="2"/>
-        <v>3.6923076923076927E-2</v>
+        <v>0</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -1902,7 +1906,7 @@
         <v>1</v>
       </c>
       <c r="D85" s="1">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
@@ -2394,6 +2398,203 @@
       </c>
       <c r="E113" t="s">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BAE116D-E1C4-504C-B7CC-C6DC99B3E159}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>